<commit_message>
update data, add waiter, namespace error
</commit_message>
<xml_diff>
--- a/aprilnames.xlsx
+++ b/aprilnames.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="13140" windowHeight="5820"/>
+    <workbookView windowWidth="19380" windowHeight="10365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="331">
   <si>
     <t>name</t>
   </si>
@@ -353,6 +353,9 @@
     <t>中国铁建房地产集团有限公司</t>
   </si>
   <si>
+    <t>中国铁建</t>
+  </si>
+  <si>
     <t>中山城建</t>
   </si>
   <si>
@@ -870,9 +873,6 @@
   </si>
   <si>
     <t>金隅集团</t>
-  </si>
-  <si>
-    <t>中国铁建</t>
   </si>
   <si>
     <t>万科企业</t>
@@ -1015,12 +1015,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1049,15 +1049,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1071,37 +1117,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1110,28 +1126,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1147,9 +1141,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1162,16 +1156,22 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1179,7 +1179,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1192,13 +1192,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1209,25 +1202,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1239,79 +1214,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1323,49 +1226,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1377,7 +1238,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1390,6 +1251,138 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1418,21 +1411,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1452,7 +1430,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1472,35 +1474,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1518,148 +1511,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2024,8 +2017,8 @@
   <sheetPr/>
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -2519,93 +2512,96 @@
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>110</v>
       </c>
       <c r="B54" t="s">
         <v>111</v>
       </c>
+      <c r="C54" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" t="s">
         <v>115</v>
-      </c>
-      <c r="C56" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
         <v>117</v>
-      </c>
-      <c r="C57" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C58" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C63" t="s">
         <v>27</v>
@@ -2613,454 +2609,454 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B64" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" t="s">
         <v>132</v>
-      </c>
-      <c r="C64" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B66" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" t="s">
         <v>136</v>
-      </c>
-      <c r="C66" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B67" t="s">
+        <v>139</v>
+      </c>
+      <c r="C67" t="s">
         <v>138</v>
-      </c>
-      <c r="C67" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C68" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" t="s">
         <v>145</v>
-      </c>
-      <c r="C70" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B71" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B72" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C74" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B75" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" t="s">
         <v>156</v>
-      </c>
-      <c r="C75" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B76" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B77" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C78" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B79" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B80" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C80" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B81" t="s">
+        <v>171</v>
+      </c>
+      <c r="C81" t="s">
         <v>170</v>
-      </c>
-      <c r="C81" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B82" t="s">
+        <v>173</v>
+      </c>
+      <c r="C82" t="s">
         <v>172</v>
-      </c>
-      <c r="C82" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B83" t="s">
+        <v>175</v>
+      </c>
+      <c r="C83" t="s">
         <v>174</v>
-      </c>
-      <c r="C83" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B84" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C84" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B85" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C85" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B86" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B87" t="s">
+        <v>185</v>
+      </c>
+      <c r="C87" t="s">
         <v>184</v>
-      </c>
-      <c r="C87" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B88" t="s">
+        <v>187</v>
+      </c>
+      <c r="C88" t="s">
         <v>186</v>
-      </c>
-      <c r="C88" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B89" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B90" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B91" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B92" t="s">
+        <v>195</v>
+      </c>
+      <c r="C92" t="s">
         <v>194</v>
-      </c>
-      <c r="C92" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B93" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B94" t="s">
+        <v>199</v>
+      </c>
+      <c r="C94" t="s">
         <v>198</v>
-      </c>
-      <c r="C94" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B95" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C95" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B96" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C96" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B97" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C97" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B98" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B99" t="s">
+        <v>212</v>
+      </c>
+      <c r="C99" t="s">
         <v>211</v>
-      </c>
-      <c r="C99" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B100" t="s">
+        <v>214</v>
+      </c>
+      <c r="C100" t="s">
         <v>213</v>
-      </c>
-      <c r="C100" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B101" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B102" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C102" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B103" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B104" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C104" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B105" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C105" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B106" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B107" t="s">
+        <v>231</v>
+      </c>
+      <c r="C107" t="s">
         <v>230</v>
-      </c>
-      <c r="C107" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B108" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B109" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C109" t="s">
         <v>99</v>
@@ -3068,153 +3064,153 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B110" t="s">
+        <v>237</v>
+      </c>
+      <c r="C110" t="s">
         <v>236</v>
-      </c>
-      <c r="C110" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B111" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C111" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B112" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B113" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C113" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B114" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B115" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B116" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B117" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B118" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B119" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B120" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B121" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B122" t="s">
+        <v>263</v>
+      </c>
+      <c r="C122" t="s">
         <v>262</v>
-      </c>
-      <c r="C122" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B123" t="s">
+        <v>265</v>
+      </c>
+      <c r="C123" t="s">
         <v>264</v>
-      </c>
-      <c r="C123" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B124" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B125" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B126" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3244,12 +3240,12 @@
     </row>
     <row r="2" ht="16.5" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:1">
@@ -3259,12 +3255,12 @@
     </row>
     <row r="5" ht="16.5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" ht="16.5" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" ht="16.5" spans="1:1">
@@ -3274,22 +3270,22 @@
     </row>
     <row r="8" ht="16.5" spans="1:1">
       <c r="A8" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" ht="16.5" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" ht="16.5" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" ht="16.5" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" ht="16.5" spans="1:1">
@@ -3314,7 +3310,7 @@
     </row>
     <row r="16" ht="16.5" spans="1:1">
       <c r="A16" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" ht="16.5" spans="1:1">
@@ -3324,7 +3320,7 @@
     </row>
     <row r="18" ht="16.5" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" ht="16.5" spans="1:1">
@@ -3334,7 +3330,7 @@
     </row>
     <row r="20" ht="16.5" spans="1:1">
       <c r="A20" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" ht="16.5" spans="1:1">
@@ -3344,17 +3340,17 @@
     </row>
     <row r="22" ht="16.5" spans="1:1">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" ht="16.5" spans="1:1">
       <c r="A23" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" ht="16.5" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" ht="16.5" spans="1:1">
@@ -3364,7 +3360,7 @@
     </row>
     <row r="26" ht="16.5" spans="1:1">
       <c r="A26" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" ht="16.5" spans="1:1">
@@ -3374,62 +3370,62 @@
     </row>
     <row r="28" ht="16.5" spans="1:1">
       <c r="A28" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" ht="16.5" spans="1:1">
       <c r="A29" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" ht="16.5" spans="1:1">
       <c r="A30" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" ht="16.5" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" ht="16.5" spans="1:1">
       <c r="A32" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" ht="16.5" spans="1:1">
       <c r="A33" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" ht="16.5" spans="1:1">
       <c r="A34" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" ht="16.5" spans="1:1">
       <c r="A35" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" ht="16.5" spans="1:1">
       <c r="A36" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" ht="16.5" spans="1:1">
       <c r="A37" s="2" t="s">
-        <v>285</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" ht="16.5" spans="1:1">
       <c r="A38" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" ht="16.5" spans="1:1">
       <c r="A39" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" ht="16.5" spans="1:1">
@@ -3439,12 +3435,12 @@
     </row>
     <row r="41" ht="16.5" spans="1:1">
       <c r="A41" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" ht="16.5" spans="1:1">
       <c r="A42" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" ht="16.5" spans="1:1">
@@ -3454,7 +3450,7 @@
     </row>
     <row r="44" ht="16.5" spans="1:1">
       <c r="A44" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" ht="16.5" spans="1:1">
@@ -3469,7 +3465,7 @@
     </row>
     <row r="47" ht="16.5" spans="1:1">
       <c r="A47" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" ht="16.5" spans="1:1">
@@ -3484,7 +3480,7 @@
     </row>
     <row r="50" ht="16.5" spans="1:1">
       <c r="A50" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="51" ht="16.5" spans="1:1">
@@ -3494,7 +3490,7 @@
     </row>
     <row r="52" ht="16.5" spans="1:1">
       <c r="A52" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" ht="16.5" spans="1:1">
@@ -3504,7 +3500,7 @@
     </row>
     <row r="54" ht="16.5" spans="1:1">
       <c r="A54" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="55" ht="16.5" spans="1:1">
@@ -3554,12 +3550,12 @@
     </row>
     <row r="64" ht="16.5" spans="1:1">
       <c r="A64" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" ht="16.5" spans="1:1">
       <c r="A65" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" ht="16.5" spans="1:1">

</xml_diff>